<commit_message>
Removed obsolete properties from TwoLayerPerceptron.
Removed LearningRate, Momentum, QuadraticRegularization.
</commit_message>
<xml_diff>
--- a/NeuralNetworks.Tests/NeuralNetworkTests.xlsx
+++ b/NeuralNetworks.Tests/NeuralNetworkTests.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="FeedForward" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="58">
   <si>
     <t>Inputs</t>
   </si>
@@ -173,6 +173,24 @@
   </si>
   <si>
     <t>Epoch 2</t>
+  </si>
+  <si>
+    <t>AdjustWeight_ShouldApplyLearningRate</t>
+  </si>
+  <si>
+    <t>AdjustWeight_ShouldApplyMomentum</t>
+  </si>
+  <si>
+    <t>Prev Gradients</t>
+  </si>
+  <si>
+    <t>AdjustWeights_ShouldApplyQuadraticRegularization</t>
+  </si>
+  <si>
+    <t>Train_OneEpoch</t>
+  </si>
+  <si>
+    <t>Train_TwoEpochsWithMomentum</t>
   </si>
 </sst>
 </file>
@@ -399,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -425,6 +443,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3375,7 +3396,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -3385,10 +3408,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:H17"/>
+  <dimension ref="B2:H36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3400,6 +3423,11 @@
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E3" s="4" t="s">
         <v>49</v>
@@ -3490,32 +3518,209 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E14" s="4" t="s">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E13" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E16" t="s">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
         <v>50</v>
       </c>
-      <c r="F16" s="22">
+      <c r="F15" s="22">
         <f>F10 - $C$4*(F7+$C$6*F10 + F7*$C$5)</f>
         <v>0.40874999999999995</v>
       </c>
-      <c r="G16" s="22">
+      <c r="G15" s="22">
         <f>G10 - $C$4*(G7+$C$6*G10 + G7*$C$5)</f>
         <v>0.81749999999999989</v>
       </c>
-      <c r="H16" s="22">
+      <c r="H15" s="22">
         <f>H10 - $C$4*(H7+$C$6*H10 + H7*$C$5)</f>
         <v>1.2262500000000001</v>
       </c>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F17" s="22">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F16" s="22">
         <f>F11 - $C$4*(F8+$C$6*F11 + F8*$C$5)</f>
         <v>-2.5962500000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="E20" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="22">
+        <f>F4 - $C$19*(F7+$C$20*F4)</f>
+        <v>0.875</v>
+      </c>
+      <c r="G20" s="22">
+        <f>G4 - $C$19*(G7+$C$20*G4)</f>
+        <v>1.75</v>
+      </c>
+      <c r="H20" s="22">
+        <f>H4 - $C$19*(H7+$C$20*H4)</f>
+        <v>2.625</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="F21" s="22">
+        <f>F5 - $C$19*(F8+$C$20*F5)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
+      <c r="E25" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="F25" s="21">
+        <v>0.3</v>
+      </c>
+      <c r="G25" s="21">
+        <v>0.4</v>
+      </c>
+      <c r="H25" s="21">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
+      <c r="F26" s="21">
+        <v>0.2</v>
+      </c>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28">
+        <v>0.5</v>
+      </c>
+      <c r="E28" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28" s="22">
+        <f>F4 - $C$28*(F7+$C$30*F4 + F25*$C$29)</f>
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="G28" s="22">
+        <f>G4 - $C$28*(G7+$C$30*G4 + G25*$C$29)</f>
+        <v>1.35</v>
+      </c>
+      <c r="H28" s="22">
+        <f>H4 - $C$28*(H7+$C$30*H4 + H25*$C$29)</f>
+        <v>2.5249999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="F29" s="22">
+        <f>F5 - $C$28*(F8+$C$30*F5 + F26*$C$29)</f>
+        <v>0.30000000000000004</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34">
+        <v>0.5</v>
+      </c>
+      <c r="E34" t="s">
+        <v>50</v>
+      </c>
+      <c r="F34" s="22">
+        <f>F4 - $C$34*(F7+$C$36*F4 + F25*$C$35)</f>
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="G34" s="22">
+        <f>G4 - $C$34*(G7+$C$36*G4 + G25*$C$35)</f>
+        <v>1.65</v>
+      </c>
+      <c r="H34" s="22">
+        <f>H4 - $C$34*(H7+$C$36*H4 + H25*$C$35)</f>
+        <v>2.4750000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="F35" s="22">
+        <f>F5 - $C$34*(F8+$C$36*F5 + F26*$C$35)</f>
+        <v>0.42500000000000004</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>